<commit_message>
added table for upgrade and fault recovery speed
</commit_message>
<xml_diff>
--- a/report/evaluations/evaluation_summary_30_08_2014.xlsx
+++ b/report/evaluations/evaluation_summary_30_08_2014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="0" windowWidth="48380" windowHeight="26500" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="520" yWindow="0" windowWidth="37720" windowHeight="26500" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="wrk data" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="89">
   <si>
     <t>30 sec</t>
   </si>
@@ -254,23 +254,50 @@
     <t>0m0.209s</t>
   </si>
   <si>
-    <t>0m0.207s</t>
-  </si>
-  <si>
     <t>INSTANT</t>
   </si>
   <si>
-    <t>0m0.208s</t>
+    <t>BAD INSTANT</t>
   </si>
   <si>
-    <t>BAD INSTANT</t>
+    <t>0m0.211s</t>
+  </si>
+  <si>
+    <t>CONCURRENT</t>
+  </si>
+  <si>
+    <t>BAD CONCURRENT</t>
+  </si>
+  <si>
+    <t>SEM</t>
+  </si>
+  <si>
+    <t>Upgrade Scenarios</t>
+  </si>
+  <si>
+    <t>INSATNT Upgrade</t>
+  </si>
+  <si>
+    <t>INSTANT Upgrade Failure</t>
+  </si>
+  <si>
+    <t>CONCURRENT Upgrade</t>
+  </si>
+  <si>
+    <t>CONCURRENT Upgrade Failure</t>
+  </si>
+  <si>
+    <t>Latency (ms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +\- SD (ms)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -314,6 +341,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="7">
@@ -564,7 +609,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="206">
+  <cellStyleXfs count="290">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -771,8 +816,92 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -879,6 +1008,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="197"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -912,9 +1042,27 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="197"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="206">
+  <cellStyles count="290">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1017,6 +1165,48 @@
     <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1119,6 +1309,48 @@
     <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="274" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="276" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="278" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="282" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="284" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="286" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="288" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="197" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1420,11 +1652,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2115320024"/>
-        <c:axId val="2115327176"/>
+        <c:axId val="-2138569544"/>
+        <c:axId val="-2138562392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2115320024"/>
+        <c:axId val="-2138569544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1486,7 +1718,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115327176"/>
+        <c:crossAx val="-2138562392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1494,7 +1726,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115327176"/>
+        <c:axId val="-2138562392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="305.0"/>
@@ -1559,7 +1791,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115320024"/>
+        <c:crossAx val="-2138569544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1937,11 +2169,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2028975848"/>
-        <c:axId val="2028099768"/>
+        <c:axId val="-2138108248"/>
+        <c:axId val="-2138100568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2028975848"/>
+        <c:axId val="-2138108248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1999,7 +2231,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028099768"/>
+        <c:crossAx val="-2138100568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2007,7 +2239,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2028099768"/>
+        <c:axId val="-2138100568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2062,7 +2294,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028975848"/>
+        <c:crossAx val="-2138108248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2153,7 +2385,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2376,11 +2607,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2028032008"/>
-        <c:axId val="2028026104"/>
+        <c:axId val="-2139074376"/>
+        <c:axId val="-2139080280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2028032008"/>
+        <c:axId val="-2139074376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2439,7 +2670,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028026104"/>
+        <c:crossAx val="-2139080280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2447,7 +2678,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2028026104"/>
+        <c:axId val="-2139080280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2512,14 +2743,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028032008"/>
+        <c:crossAx val="-2139074376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2630,7 +2860,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2849,11 +3078,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2027983848"/>
-        <c:axId val="2027977704"/>
+        <c:axId val="-2137975000"/>
+        <c:axId val="-2137968872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2027983848"/>
+        <c:axId val="-2137975000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2915,7 +3144,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2027977704"/>
+        <c:crossAx val="-2137968872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2923,7 +3152,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2027977704"/>
+        <c:axId val="-2137968872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2984,14 +3213,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2027983848"/>
+        <c:crossAx val="-2137975000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3076,7 +3304,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3299,11 +3526,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2117242520"/>
-        <c:axId val="2117248424"/>
+        <c:axId val="-2137928104"/>
+        <c:axId val="-2137922200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2117242520"/>
+        <c:axId val="-2137928104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3362,7 +3589,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2117248424"/>
+        <c:crossAx val="-2137922200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3370,7 +3597,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117248424"/>
+        <c:axId val="-2137922200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3435,14 +3662,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2117242520"/>
+        <c:crossAx val="-2137928104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3525,7 +3751,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3744,11 +3969,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2117290456"/>
-        <c:axId val="2117296344"/>
+        <c:axId val="-2137880632"/>
+        <c:axId val="-2137874728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2117290456"/>
+        <c:axId val="-2137880632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3806,7 +4031,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2117296344"/>
+        <c:crossAx val="-2137874728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3814,7 +4039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117296344"/>
+        <c:axId val="-2137874728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3869,14 +4094,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2117290456"/>
+        <c:crossAx val="-2137880632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -4214,11 +4438,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2116372008"/>
-        <c:axId val="2116377960"/>
+        <c:axId val="-2138489304"/>
+        <c:axId val="-2138483352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2116372008"/>
+        <c:axId val="-2138489304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4275,7 +4499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2116377960"/>
+        <c:crossAx val="-2138483352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4283,7 +4507,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2116377960"/>
+        <c:axId val="-2138483352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="258.0"/>
@@ -4351,7 +4575,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2116372008"/>
+        <c:crossAx val="-2138489304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="0.2"/>
@@ -4590,11 +4814,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2116429544"/>
-        <c:axId val="2116432616"/>
+        <c:axId val="-2138437096"/>
+        <c:axId val="-2138434024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2116429544"/>
+        <c:axId val="-2138437096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4604,7 +4828,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116432616"/>
+        <c:crossAx val="-2138434024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4612,7 +4836,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2116432616"/>
+        <c:axId val="-2138434024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4623,7 +4847,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116429544"/>
+        <c:crossAx val="-2138437096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4848,11 +5072,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2116465448"/>
-        <c:axId val="2116468520"/>
+        <c:axId val="-2138401192"/>
+        <c:axId val="-2138398120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2116465448"/>
+        <c:axId val="-2138401192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4862,7 +5086,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116468520"/>
+        <c:crossAx val="-2138398120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4870,7 +5094,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2116468520"/>
+        <c:axId val="-2138398120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4881,7 +5105,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116465448"/>
+        <c:crossAx val="-2138401192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5106,11 +5330,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2116499688"/>
-        <c:axId val="2116502760"/>
+        <c:axId val="-2138366952"/>
+        <c:axId val="-2138363880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2116499688"/>
+        <c:axId val="-2138366952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5120,7 +5344,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116502760"/>
+        <c:crossAx val="-2138363880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5128,7 +5352,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2116502760"/>
+        <c:axId val="-2138363880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5139,7 +5363,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116499688"/>
+        <c:crossAx val="-2138366952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5364,11 +5588,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2088258392"/>
-        <c:axId val="2088261464"/>
+        <c:axId val="-2138332296"/>
+        <c:axId val="-2138329224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2088258392"/>
+        <c:axId val="-2138332296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5378,7 +5602,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088261464"/>
+        <c:crossAx val="-2138329224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5386,7 +5610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2088261464"/>
+        <c:axId val="-2138329224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5397,7 +5621,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088258392"/>
+        <c:crossAx val="-2138332296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5759,11 +5983,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2028808952"/>
-        <c:axId val="2028816632"/>
+        <c:axId val="-2138262104"/>
+        <c:axId val="-2138254424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2028808952"/>
+        <c:axId val="-2138262104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5822,7 +6046,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028816632"/>
+        <c:crossAx val="-2138254424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5830,7 +6054,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2028816632"/>
+        <c:axId val="-2138254424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5895,7 +6119,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028808952"/>
+        <c:crossAx val="-2138262104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6288,11 +6512,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2028872440"/>
-        <c:axId val="2028880360"/>
+        <c:axId val="-2138210808"/>
+        <c:axId val="-2138202888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2028872440"/>
+        <c:axId val="-2138210808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6354,7 +6578,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028880360"/>
+        <c:crossAx val="-2138202888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6362,7 +6586,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2028880360"/>
+        <c:axId val="-2138202888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6423,7 +6647,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028872440"/>
+        <c:crossAx val="-2138210808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6812,11 +7036,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2028923608"/>
-        <c:axId val="2028931432"/>
+        <c:axId val="-2138160088"/>
+        <c:axId val="-2138152264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2028923608"/>
+        <c:axId val="-2138160088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6875,7 +7099,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028931432"/>
+        <c:crossAx val="-2138152264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6883,7 +7107,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2028931432"/>
+        <c:axId val="-2138152264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6948,7 +7172,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028923608"/>
+        <c:crossAx val="-2138160088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7798,12 +8022,12 @@
         <v>10</v>
       </c>
       <c r="N4" s="2"/>
-      <c r="O4" s="67" t="s">
+      <c r="O4" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="68"/>
+      <c r="P4" s="68"/>
+      <c r="Q4" s="68"/>
+      <c r="R4" s="69"/>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="6"/>
@@ -7843,12 +8067,12 @@
     <row r="6" spans="1:18">
       <c r="A6" s="6"/>
       <c r="B6" s="12"/>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="44"/>
       <c r="H6" s="8"/>
       <c r="I6" t="s">
@@ -7886,14 +8110,14 @@
     <row r="7" spans="1:18">
       <c r="A7" s="6"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="70" t="s">
+      <c r="D7" s="70"/>
+      <c r="E7" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="71"/>
+      <c r="F7" s="72"/>
       <c r="G7" s="14" t="s">
         <v>30</v>
       </c>
@@ -8185,12 +8409,12 @@
       <c r="G18" s="21"/>
       <c r="H18" s="22"/>
       <c r="N18" s="40"/>
-      <c r="O18" s="62" t="s">
+      <c r="O18" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="P18" s="62"/>
-      <c r="Q18" s="62"/>
-      <c r="R18" s="63"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="63"/>
+      <c r="R18" s="64"/>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="23"/>
@@ -8218,12 +8442,12 @@
     <row r="20" spans="1:18">
       <c r="A20" s="23"/>
       <c r="B20" s="26"/>
-      <c r="C20" s="62" t="s">
+      <c r="C20" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="64"/>
       <c r="G20" s="24"/>
       <c r="H20" s="25"/>
       <c r="I20" t="s">
@@ -8252,14 +8476,14 @@
     <row r="21" spans="1:18">
       <c r="A21" s="23"/>
       <c r="B21" s="27"/>
-      <c r="C21" s="64" t="s">
+      <c r="C21" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="64"/>
-      <c r="E21" s="65" t="s">
+      <c r="D21" s="65"/>
+      <c r="E21" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="66"/>
+      <c r="F21" s="67"/>
       <c r="G21" s="28" t="s">
         <v>30</v>
       </c>
@@ -8666,18 +8890,18 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="51"/>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="72"/>
-      <c r="G5" s="72" t="s">
+      <c r="D5" s="73"/>
+      <c r="G5" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="72"/>
-      <c r="K5" s="72" t="s">
+      <c r="H5" s="73"/>
+      <c r="K5" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="72"/>
+      <c r="L5" s="73"/>
       <c r="O5" s="51"/>
     </row>
     <row r="6" spans="1:15">
@@ -9033,18 +9257,18 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="40"/>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="72"/>
-      <c r="G22" s="72" t="s">
+      <c r="D22" s="73"/>
+      <c r="G22" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="72"/>
-      <c r="K22" s="72" t="s">
+      <c r="H22" s="73"/>
+      <c r="K22" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="72"/>
+      <c r="L22" s="73"/>
       <c r="O22" s="40"/>
     </row>
     <row r="23" spans="1:15">
@@ -9446,22 +9670,22 @@
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="51"/>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="72"/>
-      <c r="H4" s="72" t="s">
+      <c r="E4" s="73"/>
+      <c r="H4" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="L4" s="72" t="s">
+      <c r="I4" s="73"/>
+      <c r="L4" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="M4" s="72"/>
-      <c r="P4" s="72" t="s">
+      <c r="M4" s="73"/>
+      <c r="P4" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="Q4" s="72"/>
+      <c r="Q4" s="73"/>
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="51"/>
@@ -10125,22 +10349,22 @@
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="40"/>
-      <c r="D26" s="72" t="s">
+      <c r="D26" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="72"/>
-      <c r="H26" s="72" t="s">
+      <c r="E26" s="73"/>
+      <c r="H26" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="I26" s="72"/>
-      <c r="L26" s="72" t="s">
+      <c r="I26" s="73"/>
+      <c r="L26" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="M26" s="72"/>
-      <c r="P26" s="72" t="s">
+      <c r="M26" s="73"/>
+      <c r="P26" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="Q26" s="72"/>
+      <c r="Q26" s="73"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="40"/>
@@ -10574,22 +10798,22 @@
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="51"/>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="72"/>
-      <c r="H4" s="72" t="s">
+      <c r="E4" s="73"/>
+      <c r="H4" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="L4" s="72" t="s">
+      <c r="I4" s="73"/>
+      <c r="L4" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="M4" s="72"/>
-      <c r="P4" s="72" t="s">
+      <c r="M4" s="73"/>
+      <c r="P4" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="Q4" s="72"/>
+      <c r="Q4" s="73"/>
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="51"/>
@@ -11221,22 +11445,22 @@
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="40"/>
-      <c r="D26" s="72" t="s">
+      <c r="D26" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="72"/>
-      <c r="H26" s="72" t="s">
+      <c r="E26" s="73"/>
+      <c r="H26" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="I26" s="72"/>
-      <c r="L26" s="72" t="s">
+      <c r="I26" s="73"/>
+      <c r="L26" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="M26" s="72"/>
-      <c r="P26" s="72" t="s">
+      <c r="M26" s="73"/>
+      <c r="P26" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="Q26" s="72"/>
+      <c r="Q26" s="73"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="40"/>
@@ -11630,76 +11854,454 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B15"/>
+  <dimension ref="B3:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2">
-      <c r="B3" s="73" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2">
+    <row r="3" spans="2:11">
+      <c r="B3" s="62" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
       <c r="B4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
+        <v>78</v>
+      </c>
+      <c r="C4">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D4">
+        <f>AVERAGE(C4:C13)</f>
+        <v>4.4399999999999995E-2</v>
+      </c>
+      <c r="E4">
+        <f>(C4*1000)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
       <c r="B5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="2:2">
+      <c r="C5">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
       <c r="B6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
+        <v>74</v>
+      </c>
+      <c r="C6">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
       <c r="B7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2">
+        <v>75</v>
+      </c>
+      <c r="C7">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
       <c r="B8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2">
+        <v>74</v>
+      </c>
+      <c r="C8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
       <c r="B9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2">
+        <v>78</v>
+      </c>
+      <c r="C9">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
       <c r="B10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10">
+        <v>4.7E-2</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="11" spans="2:2">
-      <c r="B11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2">
+      <c r="C11">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="H11" s="75" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="J11" s="78"/>
+      <c r="K11" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
       <c r="B12" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="2:2">
+      <c r="C12">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="H12" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="79">
+        <v>44</v>
+      </c>
+      <c r="J12" s="78">
+        <f>_xlfn.STDEV.P(C4:C13)</f>
+        <v>1.3564659966250536E-3</v>
+      </c>
+      <c r="K12" s="79">
+        <f>(J12*1000)</f>
+        <v>1.3564659966250536</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11">
       <c r="B13" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="2:2">
-      <c r="B15" t="s">
+      <c r="C13">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="H13" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" s="80">
+        <v>45</v>
+      </c>
+      <c r="J13" s="78">
+        <f>_xlfn.STDEV.P(C16:C25)</f>
+        <v>7.4833147735478892E-4</v>
+      </c>
+      <c r="K13" s="79">
+        <f t="shared" ref="K13:K15" si="0">(J13*1000)</f>
+        <v>0.74833147735478889</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="H14" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" s="80">
+        <v>44</v>
+      </c>
+      <c r="J14" s="78">
+        <f>_xlfn.STDEV.P(C28:C36)</f>
+        <v>4.9690399499995367E-4</v>
+      </c>
+      <c r="K14" s="79">
+        <f t="shared" si="0"/>
+        <v>0.49690399499995369</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="B15" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="76" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="80">
+        <v>44</v>
+      </c>
+      <c r="J15" s="78">
+        <f>_xlfn.STDEV.P(C39:C48)</f>
+        <v>4.89897948556636E-4</v>
+      </c>
+      <c r="K15" s="79">
+        <f t="shared" si="0"/>
+        <v>0.48989794855663599</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D16">
+        <f>AVERAGE(C16:C25)</f>
+        <v>4.4199999999999989E-2</v>
+      </c>
+      <c r="E16">
+        <f>(C16*1000)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="74">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="74">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="C26" s="74"/>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="62" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D28">
+        <f>AVERAGE(C28:C37)</f>
+        <v>4.3555555555555542E-2</v>
+      </c>
+      <c r="E28">
+        <f>(C28*1000)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="C36" s="74">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="74"/>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D39">
+        <f>AVERAGE(C39:C48)</f>
+        <v>4.3599999999999986E-2</v>
+      </c>
+      <c r="E39">
+        <f>(C39*1000)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="B42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="B45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5">
+      <c r="B46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="C47" s="74">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5">
+      <c r="C48" s="74">
+        <v>4.3999999999999997E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
future plan and abstract
</commit_message>
<xml_diff>
--- a/report/evaluations/evaluation_summary_30_08_2014.xlsx
+++ b/report/evaluations/evaluation_summary_30_08_2014.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="36080" yWindow="-11120" windowWidth="39040" windowHeight="25340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="fast-feedback-graph" sheetId="8" r:id="rId1"/>
@@ -325,7 +325,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1053,6 +1052,10 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1086,10 +1089,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="292">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1538,11 +1537,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2125211992"/>
-        <c:axId val="2119043672"/>
+        <c:axId val="-2138467608"/>
+        <c:axId val="-2138440472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2125211992"/>
+        <c:axId val="-2138467608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1572,7 +1571,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2119043672"/>
+        <c:crossAx val="-2138440472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1580,7 +1579,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2119043672"/>
+        <c:axId val="-2138440472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1648,7 +1647,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125211992"/>
+        <c:crossAx val="-2138467608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1722,6 +1721,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2020,11 +2020,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2106806552"/>
-        <c:axId val="2037041976"/>
+        <c:axId val="-2133034232"/>
+        <c:axId val="-2133026408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2106806552"/>
+        <c:axId val="-2133034232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2083,7 +2083,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2037041976"/>
+        <c:crossAx val="-2133026408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2091,7 +2091,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2037041976"/>
+        <c:axId val="-2133026408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2156,13 +2156,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2106806552"/>
+        <c:crossAx val="-2133034232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2245,6 +2246,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2534,11 +2536,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2107858232"/>
-        <c:axId val="2107865912"/>
+        <c:axId val="-2132983016"/>
+        <c:axId val="-2132975336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2107858232"/>
+        <c:axId val="-2132983016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2596,7 +2598,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2107865912"/>
+        <c:crossAx val="-2132975336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2604,7 +2606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2107865912"/>
+        <c:axId val="-2132975336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2659,13 +2661,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2107858232"/>
+        <c:crossAx val="-2132983016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2973,11 +2976,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2107941720"/>
-        <c:axId val="2107947608"/>
+        <c:axId val="-2133998360"/>
+        <c:axId val="-2133992472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2107941720"/>
+        <c:axId val="-2133998360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3036,7 +3039,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2107947608"/>
+        <c:crossAx val="-2133992472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3044,7 +3047,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2107947608"/>
+        <c:axId val="-2133992472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3109,7 +3112,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2107941720"/>
+        <c:crossAx val="-2133998360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3446,11 +3449,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2107989880"/>
-        <c:axId val="2107996008"/>
+        <c:axId val="-2133950200"/>
+        <c:axId val="-2133944072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2107989880"/>
+        <c:axId val="-2133950200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3512,7 +3515,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2107996008"/>
+        <c:crossAx val="-2133944072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3520,7 +3523,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2107996008"/>
+        <c:axId val="-2133944072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3581,7 +3584,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2107989880"/>
+        <c:crossAx val="-2133950200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3896,11 +3899,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2108036776"/>
-        <c:axId val="2108042680"/>
+        <c:axId val="-2133903736"/>
+        <c:axId val="-2133897848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2108036776"/>
+        <c:axId val="-2133903736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3959,7 +3962,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108042680"/>
+        <c:crossAx val="-2133897848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3967,7 +3970,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108042680"/>
+        <c:axId val="-2133897848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4032,7 +4035,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108036776"/>
+        <c:crossAx val="-2133903736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4341,11 +4344,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2108084248"/>
-        <c:axId val="2108090152"/>
+        <c:axId val="-2134560728"/>
+        <c:axId val="-2134566616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2108084248"/>
+        <c:axId val="-2134560728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4403,7 +4406,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108090152"/>
+        <c:crossAx val="-2134566616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4411,7 +4414,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108090152"/>
+        <c:axId val="-2134566616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4466,7 +4469,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108084248"/>
+        <c:crossAx val="-2134560728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4794,11 +4797,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2077291832"/>
-        <c:axId val="2077288776"/>
+        <c:axId val="-2138077416"/>
+        <c:axId val="-2138063400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2077291832"/>
+        <c:axId val="-2138077416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4860,7 +4863,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2077288776"/>
+        <c:crossAx val="-2138063400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4868,7 +4871,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2077288776"/>
+        <c:axId val="-2138063400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="305.0"/>
@@ -4933,7 +4936,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2077291832"/>
+        <c:crossAx val="-2138077416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5277,11 +5280,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2105850472"/>
-        <c:axId val="2105856344"/>
+        <c:axId val="-2138908280"/>
+        <c:axId val="-2133357832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105850472"/>
+        <c:axId val="-2138908280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5338,7 +5341,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2105856344"/>
+        <c:crossAx val="-2133357832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5346,7 +5349,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105856344"/>
+        <c:axId val="-2133357832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="258.0"/>
@@ -5414,7 +5417,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2105850472"/>
+        <c:crossAx val="-2138908280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="0.2"/>
@@ -5653,11 +5656,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2105834520"/>
-        <c:axId val="2105826088"/>
+        <c:axId val="-2133311816"/>
+        <c:axId val="-2133308744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105834520"/>
+        <c:axId val="-2133311816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5667,7 +5670,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105826088"/>
+        <c:crossAx val="-2133308744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5675,7 +5678,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105826088"/>
+        <c:axId val="-2133308744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5686,7 +5689,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105834520"/>
+        <c:crossAx val="-2133311816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5911,11 +5914,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2105909080"/>
-        <c:axId val="2105912120"/>
+        <c:axId val="-2133275912"/>
+        <c:axId val="-2133272840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105909080"/>
+        <c:axId val="-2133275912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5925,7 +5928,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105912120"/>
+        <c:crossAx val="-2133272840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5933,7 +5936,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105912120"/>
+        <c:axId val="-2133272840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5944,7 +5947,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105909080"/>
+        <c:crossAx val="-2133275912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6169,11 +6172,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2105943192"/>
-        <c:axId val="2105946232"/>
+        <c:axId val="-2133241672"/>
+        <c:axId val="-2133238600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105943192"/>
+        <c:axId val="-2133241672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6183,7 +6186,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105946232"/>
+        <c:crossAx val="-2133238600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6191,7 +6194,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105946232"/>
+        <c:axId val="-2133238600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6202,7 +6205,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105943192"/>
+        <c:crossAx val="-2133241672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6427,11 +6430,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2105977816"/>
-        <c:axId val="2105980888"/>
+        <c:axId val="-2133207048"/>
+        <c:axId val="-2133203976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2105977816"/>
+        <c:axId val="-2133207048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6441,7 +6444,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105980888"/>
+        <c:crossAx val="-2133203976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6449,7 +6452,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2105980888"/>
+        <c:axId val="-2133203976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6460,7 +6463,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105977816"/>
+        <c:crossAx val="-2133207048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6510,7 +6513,7 @@
                 <a:latin typeface="Helvetica"/>
                 <a:cs typeface="Helvetica"/>
               </a:rPr>
-              <a:t>Absoloute Overhead Against WordPress </a:t>
+              <a:t>Absolute Overhead Against WordPress </a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="2200">
               <a:effectLst/>
@@ -6538,6 +6541,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6822,11 +6826,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2030242728"/>
-        <c:axId val="2030235240"/>
+        <c:axId val="-2133136376"/>
+        <c:axId val="-2133128696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2030242728"/>
+        <c:axId val="-2133136376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6885,7 +6889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2030235240"/>
+        <c:crossAx val="-2133128696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6893,7 +6897,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2030235240"/>
+        <c:axId val="-2133128696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6958,13 +6962,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2030242728"/>
+        <c:crossAx val="-2133136376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -7023,14 +7028,14 @@
                 <a:latin typeface="Helvetica"/>
                 <a:cs typeface="Helvetica"/>
               </a:rPr>
-              <a:t>Absoloute</a:t>
+              <a:t>Absolute </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="2200" b="1" baseline="0">
                 <a:latin typeface="Helvetica"/>
                 <a:cs typeface="Helvetica"/>
               </a:rPr>
-              <a:t> Overhead Against Couchbase </a:t>
+              <a:t>Overhead Against Couchbase </a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -7067,13 +7072,15 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -7088,13 +7095,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="0000FF"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'wordpress + couchbase 10hr'!$C$6:$C$9</c:f>
@@ -7137,7 +7138,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -7152,13 +7152,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'wordpress + couchbase 10hr'!$C$6:$C$9</c:f>
@@ -7201,7 +7195,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -7218,15 +7211,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'wordpress + couchbase 10hr'!$C$6:$C$9</c:f>
@@ -7269,7 +7254,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -7286,17 +7270,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="9"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'wordpress + couchbase 10hr'!$C$6:$C$9</c:f>
@@ -7339,7 +7313,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -7349,13 +7322,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="2030190920"/>
-        <c:axId val="2030183208"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2133085336"/>
+        <c:axId val="-2133077416"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="2030190920"/>
+        <c:axId val="-2133085336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7417,7 +7389,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2030183208"/>
+        <c:crossAx val="-2133077416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7425,7 +7397,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2030183208"/>
+        <c:axId val="-2133077416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7486,13 +7458,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2030190920"/>
+        <c:crossAx val="-2133085336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -8339,7 +8312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B8:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
@@ -8366,7 +8339,7 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="40"/>
-      <c r="C11" s="81" t="s">
+      <c r="C11" s="70" t="s">
         <v>89</v>
       </c>
       <c r="D11" s="59">
@@ -8375,7 +8348,7 @@
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="40"/>
-      <c r="C12" s="81" t="s">
+      <c r="C12" s="70" t="s">
         <v>90</v>
       </c>
       <c r="D12" s="59">
@@ -8385,7 +8358,7 @@
     </row>
     <row r="13" spans="2:4">
       <c r="B13" s="40"/>
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="70" t="s">
         <v>91</v>
       </c>
       <c r="D13" s="59">
@@ -8395,7 +8368,7 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="40"/>
-      <c r="C14" s="81" t="s">
+      <c r="C14" s="70" t="s">
         <v>92</v>
       </c>
       <c r="D14" s="59">
@@ -8405,7 +8378,7 @@
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="40"/>
-      <c r="C15" s="81" t="s">
+      <c r="C15" s="70" t="s">
         <v>93</v>
       </c>
       <c r="D15" s="59">
@@ -8415,7 +8388,7 @@
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="40"/>
-      <c r="C16" s="82" t="s">
+      <c r="C16" s="71" t="s">
         <v>94</v>
       </c>
       <c r="D16" s="59">
@@ -8425,7 +8398,7 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="40"/>
-      <c r="C17" s="82" t="s">
+      <c r="C17" s="71" t="s">
         <v>95</v>
       </c>
       <c r="D17" s="59">
@@ -8502,12 +8475,12 @@
         <v>10</v>
       </c>
       <c r="N4" s="2"/>
-      <c r="O4" s="75" t="s">
+      <c r="O4" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="75"/>
-      <c r="Q4" s="75"/>
-      <c r="R4" s="76"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="78"/>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="6"/>
@@ -8547,12 +8520,12 @@
     <row r="6" spans="1:18">
       <c r="A6" s="6"/>
       <c r="B6" s="12"/>
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="76"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="78"/>
       <c r="G6" s="44"/>
       <c r="H6" s="8"/>
       <c r="I6" t="s">
@@ -8590,14 +8563,14 @@
     <row r="7" spans="1:18">
       <c r="A7" s="6"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="77" t="s">
+      <c r="C7" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="77"/>
-      <c r="E7" s="78" t="s">
+      <c r="D7" s="79"/>
+      <c r="E7" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="79"/>
+      <c r="F7" s="81"/>
       <c r="G7" s="14" t="s">
         <v>30</v>
       </c>
@@ -8889,12 +8862,12 @@
       <c r="G18" s="21"/>
       <c r="H18" s="22"/>
       <c r="N18" s="40"/>
-      <c r="O18" s="70" t="s">
+      <c r="O18" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="P18" s="70"/>
-      <c r="Q18" s="70"/>
-      <c r="R18" s="71"/>
+      <c r="P18" s="72"/>
+      <c r="Q18" s="72"/>
+      <c r="R18" s="73"/>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="23"/>
@@ -8922,12 +8895,12 @@
     <row r="20" spans="1:18">
       <c r="A20" s="23"/>
       <c r="B20" s="26"/>
-      <c r="C20" s="70" t="s">
+      <c r="C20" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="71"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="73"/>
       <c r="G20" s="24"/>
       <c r="H20" s="25"/>
       <c r="I20" t="s">
@@ -8956,14 +8929,14 @@
     <row r="21" spans="1:18">
       <c r="A21" s="23"/>
       <c r="B21" s="27"/>
-      <c r="C21" s="72" t="s">
+      <c r="C21" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="72"/>
-      <c r="E21" s="73" t="s">
+      <c r="D21" s="74"/>
+      <c r="E21" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="74"/>
+      <c r="F21" s="76"/>
       <c r="G21" s="28" t="s">
         <v>30</v>
       </c>
@@ -9370,18 +9343,18 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="51"/>
-      <c r="C5" s="80" t="s">
+      <c r="C5" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="80"/>
-      <c r="G5" s="80" t="s">
+      <c r="D5" s="82"/>
+      <c r="G5" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="80"/>
-      <c r="K5" s="80" t="s">
+      <c r="H5" s="82"/>
+      <c r="K5" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="80"/>
+      <c r="L5" s="82"/>
       <c r="O5" s="51"/>
     </row>
     <row r="6" spans="1:15">
@@ -9737,18 +9710,18 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="40"/>
-      <c r="C22" s="80" t="s">
+      <c r="C22" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="80"/>
-      <c r="G22" s="80" t="s">
+      <c r="D22" s="82"/>
+      <c r="G22" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="80"/>
-      <c r="K22" s="80" t="s">
+      <c r="H22" s="82"/>
+      <c r="K22" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="80"/>
+      <c r="L22" s="82"/>
       <c r="O22" s="40"/>
     </row>
     <row r="23" spans="1:15">
@@ -10112,8 +10085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:S36"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="Z34" sqref="Z34"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10150,22 +10123,22 @@
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="51"/>
-      <c r="D4" s="80" t="s">
+      <c r="D4" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="H4" s="80" t="s">
+      <c r="E4" s="82"/>
+      <c r="H4" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="80"/>
-      <c r="L4" s="80" t="s">
+      <c r="I4" s="82"/>
+      <c r="L4" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="M4" s="80"/>
-      <c r="P4" s="80" t="s">
+      <c r="M4" s="82"/>
+      <c r="P4" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="Q4" s="80"/>
+      <c r="Q4" s="82"/>
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="51"/>
@@ -10829,22 +10802,22 @@
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="40"/>
-      <c r="D26" s="80" t="s">
+      <c r="D26" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="80"/>
-      <c r="H26" s="80" t="s">
+      <c r="E26" s="82"/>
+      <c r="H26" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="I26" s="80"/>
-      <c r="L26" s="80" t="s">
+      <c r="I26" s="82"/>
+      <c r="L26" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="M26" s="80"/>
-      <c r="P26" s="80" t="s">
+      <c r="M26" s="82"/>
+      <c r="P26" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="Q26" s="80"/>
+      <c r="Q26" s="82"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="40"/>
@@ -11240,7 +11213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:S36"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A35" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A36" workbookViewId="0">
       <selection activeCell="AA65" sqref="AA65"/>
     </sheetView>
   </sheetViews>
@@ -11278,22 +11251,22 @@
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="51"/>
-      <c r="D4" s="80" t="s">
+      <c r="D4" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="H4" s="80" t="s">
+      <c r="E4" s="82"/>
+      <c r="H4" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="80"/>
-      <c r="L4" s="80" t="s">
+      <c r="I4" s="82"/>
+      <c r="L4" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="M4" s="80"/>
-      <c r="P4" s="80" t="s">
+      <c r="M4" s="82"/>
+      <c r="P4" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="Q4" s="80"/>
+      <c r="Q4" s="82"/>
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="51"/>
@@ -11925,22 +11898,22 @@
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="40"/>
-      <c r="D26" s="80" t="s">
+      <c r="D26" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="80"/>
-      <c r="H26" s="80" t="s">
+      <c r="E26" s="82"/>
+      <c r="H26" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="I26" s="80"/>
-      <c r="L26" s="80" t="s">
+      <c r="I26" s="82"/>
+      <c r="L26" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="M26" s="80"/>
-      <c r="P26" s="80" t="s">
+      <c r="M26" s="82"/>
+      <c r="P26" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="Q26" s="80"/>
+      <c r="Q26" s="82"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="40"/>

</xml_diff>

<commit_message>
the report is completed and ready to print
</commit_message>
<xml_diff>
--- a/report/evaluations/evaluation_summary_30_08_2014.xlsx
+++ b/report/evaluations/evaluation_summary_30_08_2014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37980" windowHeight="26660" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="fast-feedback-graph" sheetId="8" r:id="rId1"/>
@@ -1428,7 +1428,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1537,11 +1536,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2138467608"/>
-        <c:axId val="-2138440472"/>
+        <c:axId val="-2139030056"/>
+        <c:axId val="-2139024424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2138467608"/>
+        <c:axId val="-2139030056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1571,7 +1570,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138440472"/>
+        <c:crossAx val="-2139024424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1579,7 +1578,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2138440472"/>
+        <c:axId val="-2139024424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1647,7 +1646,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138467608"/>
+        <c:crossAx val="-2139030056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2020,11 +2019,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2133034232"/>
-        <c:axId val="-2133026408"/>
+        <c:axId val="-2137488760"/>
+        <c:axId val="-2137480936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2133034232"/>
+        <c:axId val="-2137488760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2083,7 +2082,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133026408"/>
+        <c:crossAx val="-2137480936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2091,7 +2090,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133026408"/>
+        <c:axId val="-2137480936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2156,7 +2155,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133034232"/>
+        <c:crossAx val="-2137488760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2536,11 +2535,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2132983016"/>
-        <c:axId val="-2132975336"/>
+        <c:axId val="-2137437544"/>
+        <c:axId val="-2137429864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2132983016"/>
+        <c:axId val="-2137437544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2598,7 +2597,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132975336"/>
+        <c:crossAx val="-2137429864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2606,7 +2605,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132975336"/>
+        <c:axId val="-2137429864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2661,7 +2660,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132983016"/>
+        <c:crossAx val="-2137437544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2753,7 +2752,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2976,11 +2974,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2133998360"/>
-        <c:axId val="-2133992472"/>
+        <c:axId val="-2137368360"/>
+        <c:axId val="-2137362472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2133998360"/>
+        <c:axId val="-2137368360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3039,7 +3037,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133992472"/>
+        <c:crossAx val="-2137362472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3047,7 +3045,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133992472"/>
+        <c:axId val="-2137362472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3112,14 +3110,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133998360"/>
+        <c:crossAx val="-2137368360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3230,7 +3227,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3449,11 +3445,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2133950200"/>
-        <c:axId val="-2133944072"/>
+        <c:axId val="-2137320200"/>
+        <c:axId val="-2137314072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2133950200"/>
+        <c:axId val="-2137320200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3515,7 +3511,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133944072"/>
+        <c:crossAx val="-2137314072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3523,7 +3519,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133944072"/>
+        <c:axId val="-2137314072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3584,14 +3580,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133950200"/>
+        <c:crossAx val="-2137320200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3676,7 +3671,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3899,11 +3893,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2133903736"/>
-        <c:axId val="-2133897848"/>
+        <c:axId val="-2137273752"/>
+        <c:axId val="-2137267848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2133903736"/>
+        <c:axId val="-2137273752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3962,7 +3956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133897848"/>
+        <c:crossAx val="-2137267848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3970,7 +3964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133897848"/>
+        <c:axId val="-2137267848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4035,14 +4029,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133903736"/>
+        <c:crossAx val="-2137273752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -4125,7 +4118,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4344,11 +4336,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2134560728"/>
-        <c:axId val="-2134566616"/>
+        <c:axId val="-2137226280"/>
+        <c:axId val="-2137220376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2134560728"/>
+        <c:axId val="-2137226280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4406,7 +4398,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134566616"/>
+        <c:crossAx val="-2137220376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4414,7 +4406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2134566616"/>
+        <c:axId val="-2137220376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4469,14 +4461,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134560728"/>
+        <c:crossAx val="-2137226280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -4797,11 +4788,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2138077416"/>
-        <c:axId val="-2138063400"/>
+        <c:axId val="2115079272"/>
+        <c:axId val="2115073256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2138077416"/>
+        <c:axId val="2115079272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4863,7 +4854,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138063400"/>
+        <c:crossAx val="2115073256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4871,7 +4862,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2138063400"/>
+        <c:axId val="2115073256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="305.0"/>
@@ -4936,7 +4927,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138077416"/>
+        <c:crossAx val="2115079272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5280,11 +5271,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2138908280"/>
-        <c:axId val="-2133357832"/>
+        <c:axId val="2115031736"/>
+        <c:axId val="2115025768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2138908280"/>
+        <c:axId val="2115031736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5341,7 +5332,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133357832"/>
+        <c:crossAx val="2115025768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5349,7 +5340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133357832"/>
+        <c:axId val="2115025768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="258.0"/>
@@ -5417,7 +5408,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138908280"/>
+        <c:crossAx val="2115031736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="0.2"/>
@@ -5656,11 +5647,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2133311816"/>
-        <c:axId val="-2133308744"/>
+        <c:axId val="2114979608"/>
+        <c:axId val="-2137762392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2133311816"/>
+        <c:axId val="2114979608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5670,7 +5661,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133308744"/>
+        <c:crossAx val="-2137762392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5678,7 +5669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133308744"/>
+        <c:axId val="-2137762392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5689,7 +5680,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133311816"/>
+        <c:crossAx val="2114979608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5914,11 +5905,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2133275912"/>
-        <c:axId val="-2133272840"/>
+        <c:axId val="-2137729560"/>
+        <c:axId val="-2137726488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2133275912"/>
+        <c:axId val="-2137729560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5928,7 +5919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133272840"/>
+        <c:crossAx val="-2137726488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5936,7 +5927,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133272840"/>
+        <c:axId val="-2137726488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5947,7 +5938,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133275912"/>
+        <c:crossAx val="-2137729560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6172,11 +6163,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2133241672"/>
-        <c:axId val="-2133238600"/>
+        <c:axId val="-2137695112"/>
+        <c:axId val="-2137692040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2133241672"/>
+        <c:axId val="-2137695112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6186,7 +6177,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133238600"/>
+        <c:crossAx val="-2137692040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6194,7 +6185,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133238600"/>
+        <c:axId val="-2137692040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6205,7 +6196,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133241672"/>
+        <c:crossAx val="-2137695112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6430,11 +6421,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2133207048"/>
-        <c:axId val="-2133203976"/>
+        <c:axId val="-2137660488"/>
+        <c:axId val="-2137657416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2133207048"/>
+        <c:axId val="-2137660488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6444,7 +6435,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133203976"/>
+        <c:crossAx val="-2137657416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6452,7 +6443,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133203976"/>
+        <c:axId val="-2137657416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6463,7 +6454,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133207048"/>
+        <c:crossAx val="-2137660488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6826,11 +6817,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2133136376"/>
-        <c:axId val="-2133128696"/>
+        <c:axId val="-2137589752"/>
+        <c:axId val="-2137582072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2133136376"/>
+        <c:axId val="-2137589752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6889,7 +6880,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133128696"/>
+        <c:crossAx val="-2137582072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6897,7 +6888,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133128696"/>
+        <c:axId val="-2137582072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6962,7 +6953,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133136376"/>
+        <c:crossAx val="-2137589752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7078,9 +7069,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -7095,7 +7085,20 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="0000FF"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>'wordpress + couchbase 10hr'!$C$6:$C$9</c:f>
@@ -7138,6 +7141,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -7152,7 +7156,13 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>'wordpress + couchbase 10hr'!$C$6:$C$9</c:f>
@@ -7195,6 +7205,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -7211,7 +7222,15 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>'wordpress + couchbase 10hr'!$C$6:$C$9</c:f>
@@ -7254,6 +7273,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -7270,7 +7290,17 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>'wordpress + couchbase 10hr'!$C$6:$C$9</c:f>
@@ -7313,6 +7343,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -7322,12 +7353,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-2133085336"/>
-        <c:axId val="-2133077416"/>
-      </c:barChart>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2137539000"/>
+        <c:axId val="-2137532936"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="-2133085336"/>
+        <c:axId val="-2137539000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7389,7 +7421,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133077416"/>
+        <c:crossAx val="-2137532936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7397,7 +7429,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133077416"/>
+        <c:axId val="-2137532936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7458,7 +7490,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133085336"/>
+        <c:crossAx val="-2137539000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10086,7 +10118,7 @@
   <dimension ref="B3:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="I65" sqref="I65"/>
+      <selection activeCell="Y43" sqref="Y43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>